<commit_message>
added openpyxl engine support
</commit_message>
<xml_diff>
--- a/data/Tijdslijn_Maatregelen_NL.xlsx
+++ b/data/Tijdslijn_Maatregelen_NL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS\COVID-19_KM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51885CD7-A35E-4508-A549-07397038A97A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74AF4B9-2533-47DD-B2EA-1D0E12C8E47A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8772" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tijdslijn Maatregelen NL" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Datum</t>
   </si>
@@ -64,6 +64,21 @@
   </si>
   <si>
     <t>Begin studiejaar</t>
+  </si>
+  <si>
+    <t>Gedeeltelijke lockdown</t>
+  </si>
+  <si>
+    <t>Versoepelingen publieke ruimtes</t>
+  </si>
+  <si>
+    <t>Extra beperkingen op bezoekers</t>
+  </si>
+  <si>
+    <t>Mondkapjesplicht (coronawet)</t>
+  </si>
+  <si>
+    <t>Harde lockdown</t>
   </si>
 </sst>
 </file>
@@ -429,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,8 +553,48 @@
         <v>12</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>44117</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>44138</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>44152</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44179</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>